<commit_message>
moving notebook code to .py file
</commit_message>
<xml_diff>
--- a/Quora/quora_users.xlsx
+++ b/Quora/quora_users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,459 +434,659 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>user_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>is_anon</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>follower_count</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>13754147</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>24950916</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1606</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1607</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
         <v>31377999</v>
       </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
         <v>35958627</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
         <v>39308703</v>
       </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
         <v>39480350</v>
       </c>
-      <c r="B7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>146</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
         <v>39748932</v>
       </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
         <v>43887353</v>
       </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
         <v>44065510</v>
       </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
         <v>65408052</v>
       </c>
-      <c r="B11" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
         <v>24950916</v>
       </c>
-      <c r="B12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1606</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1607</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
         <v>31377999</v>
       </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
         <v>35958627</v>
       </c>
-      <c r="B14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
         <v>39308703</v>
       </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
         <v>39480350</v>
       </c>
-      <c r="B16" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>146</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
         <v>39748932</v>
       </c>
-      <c r="B17" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" t="n">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
         <v>43887353</v>
       </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
         <v>44065510</v>
       </c>
-      <c r="B19" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" t="n">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
         <v>65408052</v>
       </c>
-      <c r="B20" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" t="n">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
         <v>73403841</v>
       </c>
-      <c r="B21" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
         <v>2736</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
         <v>31377999</v>
       </c>
-      <c r="B22" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
         <v>35958627</v>
       </c>
-      <c r="B23" t="b">
-        <v>0</v>
-      </c>
-      <c r="C23" t="n">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
         <v>39308703</v>
       </c>
-      <c r="B24" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24" t="n">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
         <v>39480350</v>
       </c>
-      <c r="B25" t="b">
-        <v>0</v>
-      </c>
-      <c r="C25" t="n">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
         <v>146</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
         <v>39748932</v>
       </c>
-      <c r="B26" t="b">
-        <v>0</v>
-      </c>
-      <c r="C26" t="n">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
         <v>43887353</v>
       </c>
-      <c r="B27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" t="n">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
         <v>44065510</v>
       </c>
-      <c r="B28" t="b">
-        <v>0</v>
-      </c>
-      <c r="C28" t="n">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
         <v>65408052</v>
       </c>
-      <c r="B29" t="b">
-        <v>0</v>
-      </c>
-      <c r="C29" t="n">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
         <v>73403841</v>
       </c>
-      <c r="B30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C30" t="n">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
         <v>2736</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
         <v>82242434</v>
       </c>
-      <c r="B31" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" t="n">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>2845</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
         <v>35958627</v>
       </c>
-      <c r="B32" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" t="n">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
         <v>39308703</v>
       </c>
-      <c r="B33" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" t="n">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
         <v>39480350</v>
       </c>
-      <c r="B34" t="b">
-        <v>0</v>
-      </c>
-      <c r="C34" t="n">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
         <v>146</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
         <v>39748932</v>
       </c>
-      <c r="B35" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" t="n">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
         <v>43887353</v>
       </c>
-      <c r="B36" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" t="n">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
         <v>44065510</v>
       </c>
-      <c r="B37" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37" t="n">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
         <v>65408052</v>
       </c>
-      <c r="B38" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" t="n">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
         <v>73403841</v>
       </c>
-      <c r="B39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" t="n">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
         <v>2736</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
         <v>82242434</v>
       </c>
-      <c r="B40" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" t="n">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
         <v>2845</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
         <v>82878683</v>
       </c>
-      <c r="B41" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" t="n">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
         <v>2862</v>
       </c>
     </row>

</xml_diff>